<commit_message>
added main pages layout example
</commit_message>
<xml_diff>
--- a/data/Documents/Dashboards Design.xlsx
+++ b/data/Documents/Dashboards Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Admin Modules</t>
   </si>
@@ -84,6 +84,30 @@
   </si>
   <si>
     <t>Suggestions Tracker</t>
+  </si>
+  <si>
+    <t>API Requests total</t>
+  </si>
+  <si>
+    <t>Admins</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Book1</t>
+  </si>
+  <si>
+    <t>Api Requests</t>
+  </si>
+  <si>
+    <t>Suggestions</t>
+  </si>
+  <si>
+    <t>Book2</t>
   </si>
 </sst>
 </file>
@@ -408,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E7:E8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,86 +465,146 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test commit for wa set up
</commit_message>
<xml_diff>
--- a/data/Documents/Dashboards Design.xlsx
+++ b/data/Documents/Dashboards Design.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
+    <sheet name="Admin TODO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Admin Modules</t>
   </si>
@@ -86,9 +87,6 @@
     <t>Suggestions Tracker</t>
   </si>
   <si>
-    <t>API Requests total</t>
-  </si>
-  <si>
     <t>Admins</t>
   </si>
   <si>
@@ -101,13 +99,31 @@
     <t>Book1</t>
   </si>
   <si>
-    <t>Api Requests</t>
-  </si>
-  <si>
     <t>Suggestions</t>
   </si>
   <si>
     <t>Book2</t>
+  </si>
+  <si>
+    <t>Todo:</t>
+  </si>
+  <si>
+    <t>Bets</t>
+  </si>
+  <si>
+    <t>API Errors</t>
+  </si>
+  <si>
+    <t>API Succesful Requests</t>
+  </si>
+  <si>
+    <t>Server Exceptions (HTTP 500)</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Reports</t>
   </si>
 </sst>
 </file>
@@ -432,15 +448,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -466,146 +484,230 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>17</v>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
-        <v>26</v>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>